<commit_message>
Updated sprint plan to account for HW2
</commit_message>
<xml_diff>
--- a/project/Sprint03.xlsx
+++ b/project/Sprint03.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t xml:space="preserve">Product backlog item  </t>
   </si>
@@ -152,8 +152,15 @@
     <t>Totals</t>
   </si>
   <si>
+    <t>HW2</t>
+  </si>
+  <si>
+    <t>Do HW2</t>
+  </si>
+  <si>
     <t>Wrapped up some stuff from Sprint 1 in Sprint 2, carrying over to Sprint 3.
-Not pulling in new work, due to previous performance and mid-term season.</t>
+Not pulling in new work, due to previous performance and mid-term season.
+Added HW2 after initial planning</t>
   </si>
 </sst>
 </file>
@@ -500,25 +507,25 @@
                   <c:v>Initial Estimate of Efforts</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/9/2016</c:v>
+                  <c:v>2/16/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/10/2016</c:v>
+                  <c:v>2/17/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/11/2016</c:v>
+                  <c:v>2/18/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/12/2016</c:v>
+                  <c:v>2/19/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/13/2016</c:v>
+                  <c:v>2/20/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2/14/2016</c:v>
+                  <c:v>2/21/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2/15/2016</c:v>
+                  <c:v>2/22/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,28 +537,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -598,25 +605,25 @@
                   <c:v>Initial Estimate of Efforts</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/9/2016</c:v>
+                  <c:v>2/16/2016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/10/2016</c:v>
+                  <c:v>2/17/2016</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/11/2016</c:v>
+                  <c:v>2/18/2016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/12/2016</c:v>
+                  <c:v>2/19/2016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/13/2016</c:v>
+                  <c:v>2/20/2016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2/14/2016</c:v>
+                  <c:v>2/21/2016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2/15/2016</c:v>
+                  <c:v>2/22/2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -628,25 +635,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>12.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.714285714285714</c:v>
+                  <c:v>31.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.928571428571427</c:v>
+                  <c:v>26.071428571428569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1428571428571415</c:v>
+                  <c:v>20.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3571428571428559</c:v>
+                  <c:v>15.642857142857139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5714285714285703</c:v>
+                  <c:v>10.428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7857142857142845</c:v>
+                  <c:v>5.2142857142857091</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1736,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,25 +1778,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="7">
-        <v>42409</v>
+        <v>42416</v>
       </c>
       <c r="F1" s="7">
-        <v>42410</v>
+        <v>42417</v>
       </c>
       <c r="G1" s="7">
-        <v>42411</v>
+        <v>42418</v>
       </c>
       <c r="H1" s="7">
-        <v>42412</v>
+        <v>42419</v>
       </c>
       <c r="I1" s="7">
-        <v>42413</v>
+        <v>42420</v>
       </c>
       <c r="J1" s="7">
-        <v>42414</v>
+        <v>42421</v>
       </c>
       <c r="K1" s="7">
-        <v>42415</v>
+        <v>42422</v>
       </c>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -1806,36 +1813,36 @@
         <v>3</v>
       </c>
       <c r="D2" s="24">
-        <f>SUM(D$4:D$998)</f>
-        <v>12.5</v>
+        <f>SUM(D$4:D$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="E2" s="25">
-        <f>SUM(E$4:E$998)</f>
-        <v>12.5</v>
+        <f>SUM(E$4:E$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="F2" s="25">
-        <f>SUM(F$4:F$998)</f>
-        <v>12.5</v>
+        <f>SUM(F$4:F$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="G2" s="25">
-        <f>SUM(G$4:G$998)</f>
-        <v>12.5</v>
+        <f>SUM(G$4:G$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="H2" s="25">
-        <f>SUM(H$4:H$998)</f>
-        <v>12.5</v>
+        <f>SUM(H$4:H$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="I2" s="25">
-        <f>SUM(I$4:I$998)</f>
-        <v>12.5</v>
+        <f>SUM(I$4:I$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(J$4:J$998)</f>
-        <v>12.5</v>
+        <f>SUM(J$4:J$1001)</f>
+        <v>36.5</v>
       </c>
       <c r="K2" s="25">
-        <f>SUM(K$4:K$998)</f>
-        <v>12.5</v>
+        <f>SUM(K$4:K$1001)</f>
+        <v>36.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1846,31 +1853,31 @@
       </c>
       <c r="D3" s="24">
         <f>D2</f>
-        <v>12.5</v>
+        <v>36.5</v>
       </c>
       <c r="E3" s="25">
         <f t="shared" ref="E3:K3" si="0">D$3-$D$2/7</f>
-        <v>10.714285714285714</v>
+        <v>31.285714285714285</v>
       </c>
       <c r="F3" s="25">
         <f t="shared" si="0"/>
-        <v>8.928571428571427</v>
+        <v>26.071428571428569</v>
       </c>
       <c r="G3" s="25">
         <f t="shared" si="0"/>
-        <v>7.1428571428571415</v>
+        <v>20.857142857142854</v>
       </c>
       <c r="H3" s="25">
         <f t="shared" si="0"/>
-        <v>5.3571428571428559</v>
+        <v>15.642857142857139</v>
       </c>
       <c r="I3" s="25">
         <f t="shared" si="0"/>
-        <v>3.5714285714285703</v>
+        <v>10.428571428571423</v>
       </c>
       <c r="J3" s="25">
         <f t="shared" si="0"/>
-        <v>1.7857142857142845</v>
+        <v>5.2142857142857091</v>
       </c>
       <c r="K3" s="25">
         <f t="shared" si="0"/>
@@ -1925,8 +1932,8 @@
         <v>23</v>
       </c>
       <c r="M4">
-        <f>SUMIF(C4:C16, L4, D4:D16)</f>
-        <v>3</v>
+        <f>SUMIF(C4:C19, L4, D4:D19)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1943,7 +1950,7 @@
         <v>0.5</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:K16" si="2">D5</f>
+        <f t="shared" ref="E5:K19" si="2">D5</f>
         <v>0.5</v>
       </c>
       <c r="F5">
@@ -1974,8 +1981,8 @@
         <v>28</v>
       </c>
       <c r="M5">
-        <f>SUMIF(C5:C17, L5, D5:D17)</f>
-        <v>5</v>
+        <f>SUMIF(C5:C20, L5, D5:D20)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2023,8 +2030,8 @@
         <v>27</v>
       </c>
       <c r="M6">
-        <f>SUMIF(C6:C18, L6, D6:D18)</f>
-        <v>4</v>
+        <f>SUMIF(C6:C21, L6, D6:D21)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2293,31 +2300,31 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E13:E15" si="3">D13</f>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F13:F18" si="4">E13</f>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G13:G18" si="5">F13</f>
         <v>1</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H13:H18" si="6">G13</f>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I13:I18" si="7">H13</f>
         <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J13:J18" si="8">I13</f>
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K13:K18" si="9">J13</f>
         <v>1</v>
       </c>
     </row>
@@ -2335,31 +2342,31 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -2377,120 +2384,246 @@
         <v>0.5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B19" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A17:E21"/>
+    <mergeCell ref="A20:E24"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C4:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 C4:C19">
       <formula1>"Peter, Daniela, Jennifer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
End of 02-21 working day part way through hw2 paper abstract submitted Sprint updated
</commit_message>
<xml_diff>
--- a/project/Sprint03.xlsx
+++ b/project/Sprint03.xlsx
@@ -160,7 +160,8 @@
   <si>
     <t>Wrapped up some stuff from Sprint 1 in Sprint 2, carrying over to Sprint 3.
 Not pulling in new work, due to previous performance and mid-term season.
-Added HW2 after initial planning</t>
+Added HW2 after initial planning
+HW2 is larger than initially planned by an order of magnitude</t>
   </si>
 </sst>
 </file>
@@ -555,10 +556,10 @@
                   <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1746,7 +1747,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,36 +1814,36 @@
         <v>3</v>
       </c>
       <c r="D2" s="24">
-        <f>SUM(D$4:D$1001)</f>
+        <f t="shared" ref="D2:K2" si="0">SUM(D$4:D$1001)</f>
         <v>36.5</v>
       </c>
       <c r="E2" s="25">
-        <f>SUM(E$4:E$1001)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="F2" s="25">
-        <f>SUM(F$4:F$1001)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="G2" s="25">
-        <f>SUM(G$4:G$1001)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="H2" s="25">
-        <f>SUM(H$4:H$1001)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="I2" s="25">
-        <f>SUM(I$4:I$1001)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(J$4:J$1001)</f>
-        <v>36.5</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="K2" s="25">
-        <f>SUM(K$4:K$1001)</f>
-        <v>36.5</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1856,31 +1857,31 @@
         <v>36.5</v>
       </c>
       <c r="E3" s="25">
-        <f t="shared" ref="E3:K3" si="0">D$3-$D$2/7</f>
+        <f t="shared" ref="E3:K3" si="1">D$3-$D$2/7</f>
         <v>31.285714285714285</v>
       </c>
       <c r="F3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.071428571428569</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.857142857142854</v>
       </c>
       <c r="H3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.642857142857139</v>
       </c>
       <c r="I3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.428571428571423</v>
       </c>
       <c r="J3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2142857142857091</v>
       </c>
       <c r="K3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -1905,28 +1906,27 @@
         <v>0.5</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="1">E4</f>
+        <f t="shared" ref="F4:K4" si="2">E4</f>
         <v>0.5</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1950,32 +1950,31 @@
         <v>0.5</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:K19" si="2">D5</f>
+        <f t="shared" ref="E5:K19" si="3">D5</f>
         <v>0.5</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -1999,32 +1998,31 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
@@ -2048,32 +2046,31 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2090,31 +2087,31 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2132,31 +2129,31 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2174,31 +2171,31 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2216,31 +2213,31 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2258,31 +2255,31 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2300,31 +2297,31 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E15" si="3">D13</f>
+        <f t="shared" ref="E13:E15" si="4">D13</f>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F18" si="4">E13</f>
+        <f t="shared" ref="F13:F18" si="5">E13</f>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G18" si="5">F13</f>
+        <f t="shared" ref="G13:G18" si="6">F13</f>
         <v>1</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:H18" si="6">G13</f>
+        <f t="shared" ref="H13:H18" si="7">G13</f>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I18" si="7">H13</f>
+        <f t="shared" ref="I13:I18" si="8">H13</f>
         <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:J18" si="8">I13</f>
+        <f t="shared" ref="J13:J18" si="9">I13</f>
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13:K18" si="9">J13</f>
+        <f t="shared" ref="K13:K18" si="10">J13</f>
         <v>1</v>
       </c>
     </row>
@@ -2342,31 +2339,31 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -2384,31 +2381,31 @@
         <v>0.5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="F15">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="H15">
+      <c r="G15">
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="I15">
+      <c r="H15">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="J15">
+      <c r="I15">
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
       <c r="K15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2426,32 +2423,31 @@
         <v>8</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="G16">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="H16">
+      <c r="G16">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="I16">
+      <c r="H16">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J16">
+      <c r="I16">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
       <c r="K16">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2468,32 +2464,31 @@
         <v>8</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="H17">
+      <c r="G17">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="I17">
+      <c r="H17">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J17">
+      <c r="I17">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
       <c r="K17">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2510,32 +2505,31 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="G18">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="H18">
+      <c r="G18">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="H18">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J18">
+      <c r="I18">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
       <c r="K18">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2552,32 +2546,31 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>